<commit_message>
- On reloading lists after event executed return to last state (selected member) - Update Inmigration form memberName readonly
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/inmigration_form.xlsx
+++ b/app/src/main/res/raw/inmigration_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="26265" windowHeight="9390" tabRatio="500"/>
+    <workbookView windowWidth="28650" windowHeight="7350" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -474,10 +474,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -511,6 +511,21 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -524,6 +539,74 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -533,45 +616,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -585,72 +638,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -659,9 +646,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -693,6 +693,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -705,7 +717,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -717,31 +759,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -753,25 +831,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -783,61 +849,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -850,24 +868,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -905,15 +905,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -929,17 +920,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -962,8 +947,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -978,151 +963,166 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1480,8 +1480,8 @@
   <sheetPr/>
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
@@ -1603,7 +1603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -1622,6 +1622,9 @@
       <c r="J4" s="13"/>
       <c r="K4" s="13"/>
       <c r="L4" t="b">
+        <v>1</v>
+      </c>
+      <c r="M4" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- Update custom labels for Region reference to use the name of the hierarchy name - Fix Lowest Region Code generator
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/inmigration_form.xlsx
+++ b/app/src/main/res/raw/inmigration_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27795" windowHeight="12270" tabRatio="500"/>
+    <workbookView windowWidth="19050" windowHeight="9600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -639,10 +639,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -692,43 +692,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
@@ -736,7 +699,22 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
@@ -752,14 +730,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -774,26 +760,10 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -806,7 +776,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -820,10 +804,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF800080"/>
       <name val="Arial"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -853,187 +853,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1124,11 +1124,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1137,22 +1143,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1187,22 +1178,31 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1224,142 +1224,142 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1755,8 +1755,8 @@
   <sheetPr/>
   <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
- Add back the code for filtering member forms by age and head - Avoid nullPointerException on dataItem.getExtension().enabled of HouseholdVisitFragment - Clear custom options before adding to HForms - Fix updating Member.spouse when MaritalRelationship is created/updated
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/inmigration_form.xlsx
+++ b/app/src/main/res/raw/inmigration_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19050" windowHeight="9600" tabRatio="500"/>
+    <workbookView windowWidth="18045" windowHeight="12015" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -639,10 +639,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -676,9 +676,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="0"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -688,6 +687,52 @@
       <color theme="1"/>
       <name val="Arial"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -707,7 +752,37 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -729,17 +804,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -751,79 +820,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Arial"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -853,67 +853,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -925,115 +1033,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1124,26 +1124,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1165,44 +1156,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1221,151 +1177,195 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1755,8 +1755,8 @@
   <sheetPr/>
   <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H19"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
@@ -2955,8 +2955,8 @@
   <sheetPr/>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.18095238095238" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="3"/>

</xml_diff>